<commit_message>
Align sd-jwt and mdoc PID claims with ARF v1.8
</commit_message>
<xml_diff>
--- a/wallet-enterprise-configurations/issuer/dataset/vid-dataset.xlsx
+++ b/wallet-enterprise-configurations/issuer/dataset/vid-dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t xml:space="preserve">pid_id</t>
   </si>
@@ -37,9 +37,24 @@
     <t xml:space="preserve">issuing_country</t>
   </si>
   <si>
+    <t xml:space="preserve">age_in_years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_birth_year</t>
+  </si>
+  <si>
     <t xml:space="preserve">age_over_18</t>
   </si>
   <si>
+    <t xml:space="preserve">age_over_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_over_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_over_65</t>
+  </si>
+  <si>
     <t xml:space="preserve">family_name</t>
   </si>
   <si>
@@ -64,9 +79,36 @@
     <t xml:space="preserve">birth_place</t>
   </si>
   <si>
+    <t xml:space="preserve">birth_country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birth_region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birth_city</t>
+  </si>
+  <si>
     <t xml:space="preserve">resident_address</t>
   </si>
   <si>
+    <t xml:space="preserve">resident_country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resident_region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resident_city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resident_postal_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resident_street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resident_house_number</t>
+  </si>
+  <si>
     <t xml:space="preserve">document_number</t>
   </si>
   <si>
@@ -97,40 +139,67 @@
     <t xml:space="preserve">John</t>
   </si>
   <si>
+    <t xml:space="preserve">US,GR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New York</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manhattan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23, Random str. 34793 Apt 3 USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random str.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">john@sample.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+308388338382</t>
+  </si>
+  <si>
+    <t xml:space="preserve">john</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PID:00002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emily</t>
+  </si>
+  <si>
     <t xml:space="preserve">US</t>
   </si>
   <si>
-    <t xml:space="preserve">23, Random str. 34793 Apt 3 USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">john@sample.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+308388338382</t>
-  </si>
-  <si>
-    <t xml:space="preserve">john</t>
-  </si>
-  <si>
-    <t xml:space="preserve">secret</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PID:00002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emily</t>
-  </si>
-  <si>
     <t xml:space="preserve">24, Some str. 3473 Apt 3 USA</t>
   </si>
   <si>
+    <t xml:space="preserve">3473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some str.</t>
+  </si>
+  <si>
     <t xml:space="preserve">emily@sample.com</t>
   </si>
   <si>
     <t xml:space="preserve">emily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
   </si>
 </sst>
 </file>
@@ -276,7 +345,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -297,6 +366,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -321,7 +394,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -334,6 +407,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -374,29 +451,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:T3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:T3"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AH3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:AH3"/>
+  <tableColumns count="34">
     <tableColumn id="1" name="pid_id"/>
     <tableColumn id="2" name="issuance_date"/>
     <tableColumn id="3" name="expiry_date"/>
     <tableColumn id="4" name="issuing_authority"/>
     <tableColumn id="5" name="issuing_country"/>
-    <tableColumn id="6" name="age_over_18"/>
-    <tableColumn id="7" name="family_name"/>
-    <tableColumn id="8" name="given_name"/>
-    <tableColumn id="9" name="family_name_birth"/>
-    <tableColumn id="10" name="given_name_birth"/>
-    <tableColumn id="11" name="sex"/>
-    <tableColumn id="12" name="birth_date"/>
-    <tableColumn id="13" name="nationality"/>
-    <tableColumn id="14" name="birth_place"/>
-    <tableColumn id="15" name="resident_address"/>
-    <tableColumn id="16" name="document_number"/>
-    <tableColumn id="17" name="email_address"/>
-    <tableColumn id="18" name="mobile_phone_number"/>
-    <tableColumn id="19" name="User"/>
-    <tableColumn id="20" name="Password"/>
+    <tableColumn id="6" name="age_in_years"/>
+    <tableColumn id="7" name="age_birth_year"/>
+    <tableColumn id="8" name="age_over_18"/>
+    <tableColumn id="9" name="age_over_21"/>
+    <tableColumn id="10" name="age_over_16"/>
+    <tableColumn id="11" name="age_over_65"/>
+    <tableColumn id="12" name="family_name"/>
+    <tableColumn id="13" name="given_name"/>
+    <tableColumn id="14" name="family_name_birth"/>
+    <tableColumn id="15" name="given_name_birth"/>
+    <tableColumn id="16" name="sex"/>
+    <tableColumn id="17" name="birth_date"/>
+    <tableColumn id="18" name="nationality"/>
+    <tableColumn id="19" name="birth_place"/>
+    <tableColumn id="20" name="birth_country"/>
+    <tableColumn id="21" name="birth_region"/>
+    <tableColumn id="22" name="birth_city"/>
+    <tableColumn id="23" name="resident_address"/>
+    <tableColumn id="24" name="resident_country"/>
+    <tableColumn id="25" name="resident_region"/>
+    <tableColumn id="26" name="resident_city"/>
+    <tableColumn id="27" name="resident_postal_code"/>
+    <tableColumn id="28" name="resident_street"/>
+    <tableColumn id="29" name="resident_house_number"/>
+    <tableColumn id="30" name="document_number"/>
+    <tableColumn id="31" name="email_address"/>
+    <tableColumn id="32" name="mobile_phone_number"/>
+    <tableColumn id="33" name="User"/>
+    <tableColumn id="34" name="Password"/>
   </tableColumns>
 </table>
 </file>
@@ -406,10 +497,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:AH16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W3" activeCellId="0" sqref="W3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -419,15 +510,24 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="1" width="23.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="13" style="1" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="17.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="20" style="1" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="2" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="14" style="1" width="23.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="1" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="20" style="1" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="15.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="2" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="2" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="17.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="34" style="1" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,7 +549,7 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
@@ -476,13 +576,13 @@
       <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="7" t="s">
@@ -491,131 +591,262 @@
       <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="9" t="n">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2" s="10" t="n">
+        <v>1990</v>
+      </c>
+      <c r="H2" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="9" t="n">
+      <c r="I2" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="L2" s="10" t="n">
+      <c r="J2" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="11" t="n">
         <v>33161</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="4" t="n">
+      <c r="R2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" s="12" t="n">
+        <v>34793</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD2" s="4" t="n">
         <v>12313213</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>30</v>
+      <c r="AE2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH2" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="n">
+      <c r="A3" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="13" t="n">
+      <c r="B3" s="14"/>
+      <c r="C3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="14" t="n">
+        <v>35</v>
+      </c>
+      <c r="G3" s="14" t="n">
+        <v>1990</v>
+      </c>
+      <c r="H3" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="13" t="n">
+      <c r="I3" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="L3" s="14" t="n">
+      <c r="Q3" s="15" t="n">
         <v>33161</v>
       </c>
-      <c r="M3" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="13" t="n">
+      <c r="R3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD3" s="14" t="n">
         <v>2332131</v>
       </c>
-      <c r="Q3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>30</v>
+      <c r="AE3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D16" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" display="john@sample.com"/>
-    <hyperlink ref="Q3" r:id="rId2" display="emily@sample.com"/>
+    <hyperlink ref="AE2" r:id="rId1" display="john@sample.com"/>
+    <hyperlink ref="AE3" r:id="rId2" display="emily@sample.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
ARF 1.8 fixes and presentation definitions
</commit_message>
<xml_diff>
--- a/wallet-enterprise-configurations/issuer/dataset/vid-dataset.xlsx
+++ b/wallet-enterprise-configurations/issuer/dataset/vid-dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t xml:space="preserve">pid_id</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t xml:space="preserve">GR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
   </si>
   <si>
     <t xml:space="preserve">Doe</t>
@@ -345,7 +348,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -354,6 +357,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -394,6 +401,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -407,6 +418,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -499,8 +514,8 @@
   </sheetPr>
   <dimension ref="A1:AH16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF12" activeCellId="0" sqref="AF12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="I:K"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -512,7 +527,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="16.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="2" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="3" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="14" style="1" width="23.17"/>
@@ -521,102 +536,102 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="12.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="15.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="19.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="2" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="3" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="3" width="12.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="12.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="2" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="3" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="17.83"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="34" style="1" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AC1" s="6" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="1" t="s">
@@ -625,223 +640,223 @@
       <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AG1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="n">
+      <c r="A2" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="10" t="n">
+      <c r="F2" s="11" t="n">
         <v>35</v>
       </c>
-      <c r="G2" s="10" t="n">
+      <c r="G2" s="11" t="n">
         <v>1990</v>
       </c>
-      <c r="H2" s="12" t="n">
+      <c r="H2" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="12" t="n">
+      <c r="I2" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="12" t="n">
+      <c r="J2" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="10" t="s">
+      <c r="K2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="L2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="O2" s="10" t="s">
+      <c r="M2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="10" t="n">
+      <c r="O2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="Q2" s="11" t="n">
+      <c r="Q2" s="12" t="n">
         <v>33161</v>
       </c>
-      <c r="R2" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="11" t="s">
+      <c r="R2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="11" t="s">
+      <c r="S2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="T2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="V2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y2" s="11" t="s">
+      <c r="W2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="Z2" s="11" t="s">
+      <c r="Y2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="AA2" s="12" t="n">
+      <c r="Z2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="14" t="n">
         <v>34793</v>
       </c>
-      <c r="AB2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AB2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="AD2" s="4" t="n">
+      <c r="AC2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD2" s="5" t="n">
         <v>12313213</v>
       </c>
-      <c r="AE2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AG2" s="10" t="s">
+      <c r="AF2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="AH2" s="10" t="s">
+      <c r="AG2" s="11" t="s">
         <v>49</v>
+      </c>
+      <c r="AH2" s="11" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="16" t="n">
+        <v>35</v>
+      </c>
+      <c r="G3" s="16" t="n">
+        <v>1990</v>
+      </c>
+      <c r="H3" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="17" t="n">
+        <v>33161</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="S3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="V3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="W3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="X3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD3" s="16" t="n">
+        <v>2332131</v>
+      </c>
+      <c r="AE3" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH3" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="14" t="n">
-        <v>35</v>
-      </c>
-      <c r="G3" s="14" t="n">
-        <v>1990</v>
-      </c>
-      <c r="H3" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="P3" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="15" t="n">
-        <v>33161</v>
-      </c>
-      <c r="R3" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="S3" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="T3" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="V3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="W3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="X3" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB3" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC3" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD3" s="14" t="n">
-        <v>2332131</v>
-      </c>
-      <c r="AE3" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG3" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH3" s="10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add missing fields on PID and presentation definitions
</commit_message>
<xml_diff>
--- a/wallet-enterprise-configurations/issuer/dataset/vid-dataset.xlsx
+++ b/wallet-enterprise-configurations/issuer/dataset/vid-dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t xml:space="preserve">pid_id</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">issuing_country</t>
   </si>
   <si>
+    <t xml:space="preserve">issuing_jurisdiction</t>
+  </si>
+  <si>
     <t xml:space="preserve">age_in_years</t>
   </si>
   <si>
@@ -118,6 +121,9 @@
     <t xml:space="preserve">mobile_phone_number</t>
   </si>
   <si>
+    <t xml:space="preserve">personal_administrative_number</t>
+  </si>
+  <si>
     <t xml:space="preserve">User</t>
   </si>
   <si>
@@ -133,6 +139,9 @@
     <t xml:space="preserve">GR</t>
   </si>
   <si>
+    <t xml:space="preserve">GR-F</t>
+  </si>
+  <si>
     <t xml:space="preserve">0</t>
   </si>
   <si>
@@ -169,6 +178,9 @@
     <t xml:space="preserve">+308388338382</t>
   </si>
   <si>
+    <t xml:space="preserve">123456789</t>
+  </si>
+  <si>
     <t xml:space="preserve">john</t>
   </si>
   <si>
@@ -197,6 +209,9 @@
   </si>
   <si>
     <t xml:space="preserve">emily@sample.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">987654321</t>
   </si>
   <si>
     <t xml:space="preserve">emily</t>
@@ -216,7 +231,7 @@
     <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -253,6 +268,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -348,7 +369,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,10 +378,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -401,7 +418,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -421,7 +438,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -466,43 +483,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AH3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:AH3"/>
-  <tableColumns count="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AJ3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:AJ3"/>
+  <tableColumns count="36">
     <tableColumn id="1" name="pid_id"/>
     <tableColumn id="2" name="issuance_date"/>
     <tableColumn id="3" name="expiry_date"/>
     <tableColumn id="4" name="issuing_authority"/>
     <tableColumn id="5" name="issuing_country"/>
-    <tableColumn id="6" name="age_in_years"/>
-    <tableColumn id="7" name="age_birth_year"/>
-    <tableColumn id="8" name="age_over_18"/>
-    <tableColumn id="9" name="age_over_21"/>
-    <tableColumn id="10" name="age_over_16"/>
-    <tableColumn id="11" name="age_over_65"/>
-    <tableColumn id="12" name="family_name"/>
-    <tableColumn id="13" name="given_name"/>
-    <tableColumn id="14" name="family_name_birth"/>
-    <tableColumn id="15" name="given_name_birth"/>
-    <tableColumn id="16" name="sex"/>
-    <tableColumn id="17" name="birth_date"/>
-    <tableColumn id="18" name="nationality"/>
-    <tableColumn id="19" name="birth_place"/>
-    <tableColumn id="20" name="birth_country"/>
-    <tableColumn id="21" name="birth_region"/>
-    <tableColumn id="22" name="birth_city"/>
-    <tableColumn id="23" name="resident_address"/>
-    <tableColumn id="24" name="resident_country"/>
-    <tableColumn id="25" name="resident_region"/>
-    <tableColumn id="26" name="resident_city"/>
-    <tableColumn id="27" name="resident_postal_code"/>
-    <tableColumn id="28" name="resident_street"/>
-    <tableColumn id="29" name="resident_house_number"/>
-    <tableColumn id="30" name="document_number"/>
-    <tableColumn id="31" name="email_address"/>
-    <tableColumn id="32" name="mobile_phone_number"/>
-    <tableColumn id="33" name="User"/>
-    <tableColumn id="34" name="Password"/>
+    <tableColumn id="6" name="issuing_jurisdiction"/>
+    <tableColumn id="7" name="age_in_years"/>
+    <tableColumn id="8" name="age_birth_year"/>
+    <tableColumn id="9" name="age_over_18"/>
+    <tableColumn id="10" name="age_over_21"/>
+    <tableColumn id="11" name="age_over_16"/>
+    <tableColumn id="12" name="age_over_65"/>
+    <tableColumn id="13" name="family_name"/>
+    <tableColumn id="14" name="given_name"/>
+    <tableColumn id="15" name="family_name_birth"/>
+    <tableColumn id="16" name="given_name_birth"/>
+    <tableColumn id="17" name="sex"/>
+    <tableColumn id="18" name="birth_date"/>
+    <tableColumn id="19" name="nationality"/>
+    <tableColumn id="20" name="birth_place"/>
+    <tableColumn id="21" name="birth_country"/>
+    <tableColumn id="22" name="birth_region"/>
+    <tableColumn id="23" name="birth_city"/>
+    <tableColumn id="24" name="resident_address"/>
+    <tableColumn id="25" name="resident_country"/>
+    <tableColumn id="26" name="resident_region"/>
+    <tableColumn id="27" name="resident_city"/>
+    <tableColumn id="28" name="resident_postal_code"/>
+    <tableColumn id="29" name="resident_street"/>
+    <tableColumn id="30" name="resident_house_number"/>
+    <tableColumn id="31" name="document_number"/>
+    <tableColumn id="32" name="email_address"/>
+    <tableColumn id="33" name="mobile_phone_number"/>
+    <tableColumn id="34" name="personal_administrative_number"/>
+    <tableColumn id="35" name="User"/>
+    <tableColumn id="36" name="Password"/>
   </tableColumns>
 </table>
 </file>
@@ -512,357 +531,373 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AH16"/>
+  <dimension ref="A1:AJ16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="I:K"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="3" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="14" style="1" width="23.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="1" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="20" style="1" width="27.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="15.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="3" width="19.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="3" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="3" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="17.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="34" style="1" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="1" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="2" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="15" style="1" width="23.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="1" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="21" style="1" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="15.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="2" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="2" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="17.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="36" style="1" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="5" t="s">
         <v>29</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="AI1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="n">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="H2" s="10" t="n">
+        <v>1990</v>
+      </c>
+      <c r="I2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" s="11" t="n">
+        <v>33161</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB2" s="13" t="n">
+        <v>34793</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE2" s="4" t="n">
+        <v>12313213</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ2" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="11" t="n">
+      <c r="D3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="15" t="n">
         <v>35</v>
       </c>
-      <c r="G2" s="11" t="n">
+      <c r="H3" s="15" t="n">
         <v>1990</v>
       </c>
-      <c r="H2" s="13" t="n">
+      <c r="I3" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="14" t="n">
+      <c r="J3" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="14" t="n">
+      <c r="K3" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="12" t="n">
+      <c r="L3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q3" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="R3" s="16" t="n">
         <v>33161</v>
       </c>
-      <c r="R2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="W2" s="12" t="s">
+      <c r="S3" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="X2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA2" s="14" t="n">
-        <v>34793</v>
-      </c>
-      <c r="AB2" s="14" t="s">
+      <c r="U3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="AC2" s="14" t="s">
+      <c r="W3" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="AD2" s="5" t="n">
-        <v>12313213</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG2" s="11" t="s">
+      <c r="X3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD3" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="AH2" s="11" t="s">
-        <v>50</v>
+      <c r="AE3" s="15" t="n">
+        <v>2332131</v>
+      </c>
+      <c r="AF3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="16" t="n">
-        <v>35</v>
-      </c>
-      <c r="G3" s="16" t="n">
-        <v>1990</v>
-      </c>
-      <c r="H3" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="P3" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="17" t="n">
-        <v>33161</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="S3" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="T3" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="U3" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="V3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="W3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="X3" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y3" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA3" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB3" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD3" s="16" t="n">
-        <v>2332131</v>
-      </c>
-      <c r="AE3" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH3" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AE2" r:id="rId1" display="john@sample.com"/>
-    <hyperlink ref="AE3" r:id="rId2" display="emily@sample.com"/>
+    <hyperlink ref="AF2" r:id="rId1" display="john@sample.com"/>
+    <hyperlink ref="AF3" r:id="rId2" display="emily@sample.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Change addresses in pid dataset, change labels on verifier
</commit_message>
<xml_diff>
--- a/wallet-enterprise-configurations/issuer/dataset/vid-dataset.xlsx
+++ b/wallet-enterprise-configurations/issuer/dataset/vid-dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
   <si>
     <t xml:space="preserve">pid_id</t>
   </si>
@@ -157,9 +157,6 @@
     <t xml:space="preserve">US,GR</t>
   </si>
   <si>
-    <t xml:space="preserve">USA</t>
-  </si>
-  <si>
     <t xml:space="preserve">US</t>
   </si>
   <si>
@@ -169,7 +166,8 @@
     <t xml:space="preserve">Manhattan</t>
   </si>
   <si>
-    <t xml:space="preserve">23, Random str. 34793 Apt 3 USA</t>
+    <t xml:space="preserve">Random str. 3, 34793 Manhattan, New York, US
+</t>
   </si>
   <si>
     <t xml:space="preserve">Random str.</t>
@@ -202,7 +200,7 @@
     <t xml:space="preserve">Emily</t>
   </si>
   <si>
-    <t xml:space="preserve">24, Some str. 3473 Apt 3 USA</t>
+    <t xml:space="preserve">Some str. 3, 3473 Manhattan, New York, US</t>
   </si>
   <si>
     <t xml:space="preserve">3473</t>
@@ -265,18 +263,18 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -372,7 +370,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -393,10 +391,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -409,7 +403,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,6 +421,14 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -533,8 +535,8 @@
   </sheetPr>
   <dimension ref="A1:AK16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y15" activeCellId="0" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -588,73 +590,73 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="5" t="s">
         <v>30</v>
       </c>
       <c r="AF1" s="1" t="s">
@@ -669,238 +671,238 @@
       <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="9" t="s">
+      <c r="AK1" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12" t="s">
+    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="11" t="n">
+      <c r="G2" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="H2" s="11" t="n">
+      <c r="H2" s="10" t="n">
         <v>1990</v>
       </c>
-      <c r="I2" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="13" t="s">
+      <c r="I2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="P2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" s="12" t="n">
+      <c r="R2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" s="11" t="n">
         <v>33161</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="T2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="U2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="V2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="12" t="s">
+      <c r="X2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="Y2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="12" t="s">
+      <c r="Z2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC2" s="12" t="n">
+        <v>34793</v>
+      </c>
+      <c r="AD2" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC2" s="13" t="n">
-        <v>34793</v>
-      </c>
-      <c r="AD2" s="13" t="s">
+      <c r="AE2" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>51</v>
       </c>
       <c r="AF2" s="4" t="n">
         <v>12313213</v>
       </c>
       <c r="AG2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="AJ2" s="11" t="s">
+      <c r="AK2" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="AK2" s="11" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="n">
+      <c r="A3" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="16" t="n">
+        <v>35</v>
+      </c>
+      <c r="H3" s="16" t="n">
+        <v>1990</v>
+      </c>
+      <c r="I3" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="15" t="n">
-        <v>35</v>
-      </c>
-      <c r="H3" s="15" t="n">
-        <v>1990</v>
-      </c>
-      <c r="I3" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="P3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="R3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="S3" s="17" t="n">
+        <v>33161</v>
+      </c>
+      <c r="T3" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y3" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="R3" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="S3" s="16" t="n">
-        <v>33161</v>
-      </c>
-      <c r="T3" s="16" t="s">
+      <c r="Z3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA3" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="V3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="W3" s="12" t="s">
+      <c r="AB3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="X3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y3" s="12" t="s">
+      <c r="AC3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="Z3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA3" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC3" s="13" t="s">
+      <c r="AD3" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AD3" s="13" t="s">
+      <c r="AE3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF3" s="16" t="n">
+        <v>2332131</v>
+      </c>
+      <c r="AG3" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="AE3" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF3" s="15" t="n">
-        <v>2332131</v>
-      </c>
-      <c r="AG3" s="15" t="s">
+      <c r="AH3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AH3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI3" s="6" t="s">
+      <c r="AJ3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AJ3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="AK3" s="11" t="s">
-        <v>56</v>
+      <c r="AK3" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>